<commit_message>
added pyclassUnit sheet to excel commands
</commit_message>
<xml_diff>
--- a/processing/commands.xlsx
+++ b/processing/commands.xlsx
@@ -5,22 +5,27 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\python\ESRI\Reprojection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\python\ESRI\Translate\processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="6345"/>
   </bookViews>
   <sheets>
-    <sheet name="copy_parcel_files2cypress" sheetId="8" r:id="rId1"/>
-    <sheet name="copy_parcel_files2local" sheetId="6" r:id="rId2"/>
-    <sheet name="scratch" sheetId="7" r:id="rId3"/>
-    <sheet name="reproject_parcels" sheetId="1" r:id="rId4"/>
-    <sheet name="reproject_parcelsplus" sheetId="4" r:id="rId5"/>
-    <sheet name="make_directory_in_S" sheetId="9" r:id="rId6"/>
-    <sheet name="make_directory" sheetId="3" r:id="rId7"/>
-    <sheet name="lists" sheetId="2" r:id="rId8"/>
+    <sheet name="pyclassUnit" sheetId="11" r:id="rId1"/>
+    <sheet name="copy_parcel_files2cypress" sheetId="8" r:id="rId2"/>
+    <sheet name="copy_parcel_files2local" sheetId="6" r:id="rId3"/>
+    <sheet name="scratch" sheetId="7" r:id="rId4"/>
+    <sheet name="reproject_parcels" sheetId="1" r:id="rId5"/>
+    <sheet name="reproject_parcelsplus" sheetId="4" r:id="rId6"/>
+    <sheet name="make_directory_in_S" sheetId="9" r:id="rId7"/>
+    <sheet name="make_directory" sheetId="3" r:id="rId8"/>
+    <sheet name="lists" sheetId="2" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="UnitList" localSheetId="8">lists!$F$1:$M$34</definedName>
+    <definedName name="UnitList" localSheetId="0">pyclassUnit!$D$1:$J$34</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,8 +35,39 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="UnitList1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="UnitList11" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7227" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="871">
   <si>
     <t>01AlleganTwp</t>
   </si>
@@ -2101,6 +2137,549 @@
   </si>
   <si>
     <t>copy J:\Apps\Products\AccuGlobe\LocalUnits\build\59DouglasCity\IntlFt\Parcels.sbx S:\Secure\Units\DouglasCity\LIS\IntlFt\Parcels.sbx</t>
+  </si>
+  <si>
+    <t>Monterey Twp</t>
+  </si>
+  <si>
+    <t>T3N  R13W</t>
+  </si>
+  <si>
+    <t>Monterey Township</t>
+  </si>
+  <si>
+    <t>Monterey</t>
+  </si>
+  <si>
+    <t>Township</t>
+  </si>
+  <si>
+    <t>Otsego City</t>
+  </si>
+  <si>
+    <t>Otsego</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Gun Plain Twp</t>
+  </si>
+  <si>
+    <t>T1N  R11W</t>
+  </si>
+  <si>
+    <t>Gun Plain Township</t>
+  </si>
+  <si>
+    <t>Gun Plain</t>
+  </si>
+  <si>
+    <t>Salem Twp</t>
+  </si>
+  <si>
+    <t>T4N  R13W</t>
+  </si>
+  <si>
+    <t>Salem Township</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Heath Twp</t>
+  </si>
+  <si>
+    <t>T3N  R14W</t>
+  </si>
+  <si>
+    <t>Heath Township</t>
+  </si>
+  <si>
+    <t>Heath</t>
+  </si>
+  <si>
+    <t>Allegan City</t>
+  </si>
+  <si>
+    <t>Allegan</t>
+  </si>
+  <si>
+    <t>Allegan Twp</t>
+  </si>
+  <si>
+    <t>T2N  R13W</t>
+  </si>
+  <si>
+    <t>Allegan Township</t>
+  </si>
+  <si>
+    <t>Trowbridge Twp</t>
+  </si>
+  <si>
+    <t>T1N  R13W</t>
+  </si>
+  <si>
+    <t>Trowbridge Township</t>
+  </si>
+  <si>
+    <t>Trowbridge</t>
+  </si>
+  <si>
+    <t>Watson Twp</t>
+  </si>
+  <si>
+    <t>T2N  R12W</t>
+  </si>
+  <si>
+    <t>Watson Township</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>Dorr Twp</t>
+  </si>
+  <si>
+    <t>T4N  R12W</t>
+  </si>
+  <si>
+    <t>Dorr Township</t>
+  </si>
+  <si>
+    <t>Dorr</t>
+  </si>
+  <si>
+    <t>Overisel Twp</t>
+  </si>
+  <si>
+    <t>T4N  R14W</t>
+  </si>
+  <si>
+    <t>Overisel Township</t>
+  </si>
+  <si>
+    <t>Overisel</t>
+  </si>
+  <si>
+    <t>Valley Twp</t>
+  </si>
+  <si>
+    <t>T2N  R14W</t>
+  </si>
+  <si>
+    <t>Valley Township</t>
+  </si>
+  <si>
+    <t>Valley</t>
+  </si>
+  <si>
+    <t>Cheshire Twp</t>
+  </si>
+  <si>
+    <t>T1N  R14W</t>
+  </si>
+  <si>
+    <t>Cheshire Township</t>
+  </si>
+  <si>
+    <t>Cheshire</t>
+  </si>
+  <si>
+    <t>Lee Twp</t>
+  </si>
+  <si>
+    <t>T1N  R15W</t>
+  </si>
+  <si>
+    <t>Lee Township</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Martin Village</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Martin Twp</t>
+  </si>
+  <si>
+    <t>T2N  R11W</t>
+  </si>
+  <si>
+    <t>Martin Township</t>
+  </si>
+  <si>
+    <t>Hopkins Village</t>
+  </si>
+  <si>
+    <t>Hopkins</t>
+  </si>
+  <si>
+    <t>Hopkins Twp</t>
+  </si>
+  <si>
+    <t>T3N  R12W</t>
+  </si>
+  <si>
+    <t>Hopkins Township</t>
+  </si>
+  <si>
+    <t>Wayland City</t>
+  </si>
+  <si>
+    <t>Wayland</t>
+  </si>
+  <si>
+    <t>Wayland Twp</t>
+  </si>
+  <si>
+    <t>T3N  R11W</t>
+  </si>
+  <si>
+    <t>Wayland Township</t>
+  </si>
+  <si>
+    <t>Leighton Twp</t>
+  </si>
+  <si>
+    <t>T4N  R11W</t>
+  </si>
+  <si>
+    <t>Leighton Township</t>
+  </si>
+  <si>
+    <t>Leighton</t>
+  </si>
+  <si>
+    <t>Fennville City</t>
+  </si>
+  <si>
+    <t>Fennville</t>
+  </si>
+  <si>
+    <t>Manlius Twp</t>
+  </si>
+  <si>
+    <t>T3N  R15W</t>
+  </si>
+  <si>
+    <t>Manlius Township</t>
+  </si>
+  <si>
+    <t>Manlius</t>
+  </si>
+  <si>
+    <t>Clyde Twp</t>
+  </si>
+  <si>
+    <t>T2N  R15W</t>
+  </si>
+  <si>
+    <t>Clyde Township</t>
+  </si>
+  <si>
+    <t>Clyde</t>
+  </si>
+  <si>
+    <t>Plainwell City</t>
+  </si>
+  <si>
+    <t>Plainwell</t>
+  </si>
+  <si>
+    <t>Otsego Twp</t>
+  </si>
+  <si>
+    <t>T1N  R12W</t>
+  </si>
+  <si>
+    <t>Otsego Township</t>
+  </si>
+  <si>
+    <t>Laketown Twp</t>
+  </si>
+  <si>
+    <t>T4N  R16W</t>
+  </si>
+  <si>
+    <t>Laketown Township</t>
+  </si>
+  <si>
+    <t>Laketown</t>
+  </si>
+  <si>
+    <t>Douglas City</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Ganges Twp</t>
+  </si>
+  <si>
+    <t>T2N  R16W</t>
+  </si>
+  <si>
+    <t>Ganges Township</t>
+  </si>
+  <si>
+    <t>Ganges</t>
+  </si>
+  <si>
+    <t>South Haven City</t>
+  </si>
+  <si>
+    <t>South Haven</t>
+  </si>
+  <si>
+    <t>Casco Twp</t>
+  </si>
+  <si>
+    <t>T1N  R16W</t>
+  </si>
+  <si>
+    <t>Casco Township</t>
+  </si>
+  <si>
+    <t>Casco</t>
+  </si>
+  <si>
+    <t>Fillmore Twp</t>
+  </si>
+  <si>
+    <t>T4N  R15W</t>
+  </si>
+  <si>
+    <t>Fillmore Township</t>
+  </si>
+  <si>
+    <t>Fillmore</t>
+  </si>
+  <si>
+    <t>Saugatuck Twp</t>
+  </si>
+  <si>
+    <t>T3N  R16W</t>
+  </si>
+  <si>
+    <t>Saugatuck Township</t>
+  </si>
+  <si>
+    <t>Saugatucl</t>
+  </si>
+  <si>
+    <t>Saugatuck City</t>
+  </si>
+  <si>
+    <t>Saugatuck</t>
+  </si>
+  <si>
+    <t>Holland City</t>
+  </si>
+  <si>
+    <t>Holland</t>
+  </si>
+  <si>
+    <t>South HavenCity</t>
+  </si>
+  <si>
+    <t>HollandCity</t>
+  </si>
+  <si>
+    <t>01260</t>
+  </si>
+  <si>
+    <t>01280</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>T2NR13W</t>
+  </si>
+  <si>
+    <t>T1NR16W</t>
+  </si>
+  <si>
+    <t>T1NR14W</t>
+  </si>
+  <si>
+    <t>T2NR15W</t>
+  </si>
+  <si>
+    <t>T4NR12W</t>
+  </si>
+  <si>
+    <t>T4NR15W</t>
+  </si>
+  <si>
+    <t>T2NR16W</t>
+  </si>
+  <si>
+    <t>T1NR11W</t>
+  </si>
+  <si>
+    <t>T3NR14W</t>
+  </si>
+  <si>
+    <t>T3NR12W</t>
+  </si>
+  <si>
+    <t>T4NR16W</t>
+  </si>
+  <si>
+    <t>T1NR15W</t>
+  </si>
+  <si>
+    <t>T4NR11W</t>
+  </si>
+  <si>
+    <t>T3NR15W</t>
+  </si>
+  <si>
+    <t>T2NR11W</t>
+  </si>
+  <si>
+    <t>T3NR13W</t>
+  </si>
+  <si>
+    <t>T1NR12W</t>
+  </si>
+  <si>
+    <t>T4NR14W</t>
+  </si>
+  <si>
+    <t>T4NR13W</t>
+  </si>
+  <si>
+    <t>T3NR16W</t>
+  </si>
+  <si>
+    <t>T1NR13W</t>
+  </si>
+  <si>
+    <t>T2NR14W</t>
+  </si>
+  <si>
+    <t>T2NR12W</t>
+  </si>
+  <si>
+    <t>T3NR11W</t>
+  </si>
+  <si>
+    <t>unit01 = Unit("01","01280","Allegan Twp","AlleganTwp","T2NR13W",Allegan Township",Allegan",Township")</t>
+  </si>
+  <si>
+    <t>unit02 = Unit("02","13700","Casco Twp","CascoTwp","T1NR16W",Casco Township",Casco",Township")</t>
+  </si>
+  <si>
+    <t>unit03 = Unit("03","15200","Cheshire Twp","CheshireTwp","T1NR14W",Cheshire Township",Cheshire",Township")</t>
+  </si>
+  <si>
+    <t>unit04 = Unit("04","16720","Clyde Twp","ClydeTwp","T2NR15W",Clyde Township",Clyde",Township")</t>
+  </si>
+  <si>
+    <t>unit05 = Unit("05","22680","Dorr Twp","DorrTwp","T4NR12W",Dorr Township",Dorr",Township")</t>
+  </si>
+  <si>
+    <t>unit06 = Unit("06","28120","Fillmore Twp","FillmoreTwp","T4NR15W",Fillmore Township",Fillmore",Township")</t>
+  </si>
+  <si>
+    <t>unit07 = Unit("07","31360","Ganges Twp","GangesTwp","T2NR16W",Ganges Township",Ganges",Township")</t>
+  </si>
+  <si>
+    <t>unit08 = Unit("08","35720","Gun Plain Twp","GunPlainTwp","T1NR11W",Gun Plain Township",Gun Plain",Township")</t>
+  </si>
+  <si>
+    <t>unit09 = Unit("09","37460","Heath Twp","HeathTwp","T3NR14W",Heath Township",Heath",Township")</t>
+  </si>
+  <si>
+    <t>unit10 = Unit("10","39200","Hopkins Twp","HopkinsTwp","T3NR12W",Hopkins Township",Hopkins",Township")</t>
+  </si>
+  <si>
+    <t>unit11 = Unit("11","45180","Laketown Twp","LaketownTwp","T4NR16W",Laketown Township",Laketown",Township")</t>
+  </si>
+  <si>
+    <t>unit12 = Unit("12","46600","Lee Twp","LeeTwp","T1NR15W",Lee Township",Lee",Township")</t>
+  </si>
+  <si>
+    <t>unit13 = Unit("13","46760","Leighton Twp","LeightonTwp","T4NR11W",Leighton Township",Leighton",Township")</t>
+  </si>
+  <si>
+    <t>unit14 = Unit("14","50840","Manlius Twp","ManliusTwp","T3NR15W",Manlius Township",Manlius",Township")</t>
+  </si>
+  <si>
+    <t>unit15 = Unit("15","52000","Martin Twp","MartinTwp","T2NR11W",Martin Township",Martin",Township")</t>
+  </si>
+  <si>
+    <t>unit16 = Unit("16","55200","Monterey Twp","MontereyTwp","T3NR13W",Monterey Township",Monterey",Township")</t>
+  </si>
+  <si>
+    <t>unit17 = Unit("17","61640","Otsego Twp","OtsegoTwp","T1NR12W",Otsego Township",Otsego",Township")</t>
+  </si>
+  <si>
+    <t>unit18 = Unit("18","61820","Overisel Twp","OveriselTwp","T4NR14W",Overisel Township",Overisel",Township")</t>
+  </si>
+  <si>
+    <t>unit19 = Unit("19","71100","Salem Twp","SalemTwp","T4NR13W",Salem Township",Salem",Township")</t>
+  </si>
+  <si>
+    <t>unit20 = Unit("20","71720","Saugatuck Twp","SaugatuckTwp","T3NR16W",Saugatuck Township",Saugatucl",Township")</t>
+  </si>
+  <si>
+    <t>unit21 = Unit("21","80620","Trowbridge Twp","TrowbridgeTwp","T1NR13W",Trowbridge Township",Trowbridge",Township")</t>
+  </si>
+  <si>
+    <t>unit22 = Unit("22","81580","Valley Twp","ValleyTwp","T2NR14W",Valley Township",Valley",Township")</t>
+  </si>
+  <si>
+    <t>unit23 = Unit("23","84580","Watson Twp","WatsonTwp","T2NR12W",Watson Township",Watson",Township")</t>
+  </si>
+  <si>
+    <t>unit24 = Unit("24","84900","Wayland Twp","WaylandTwp","T3NR11W",Wayland Township",Wayland",Township")</t>
+  </si>
+  <si>
+    <t>unit42 = Unit("42","39200","Hopkins Village","Hopkins Village","",Hopkins Village",Hopkins",Village")</t>
+  </si>
+  <si>
+    <t>unit44 = Unit("44","52000","Martin Village","Martin Village","",Martin Village",Martin",Village")</t>
+  </si>
+  <si>
+    <t>unit51 = Unit("51","01260","Allegan City","AlleganCity","",Allegan City",Allegan",City")</t>
+  </si>
+  <si>
+    <t>unit52 = Unit("52","27740","Fennville City","FennvilleCity","",Fennville City",Fennville",City")</t>
+  </si>
+  <si>
+    <t>unit53 = Unit("53","38640","Holland City","HollandCity","",Holland City",Holland",City")</t>
+  </si>
+  <si>
+    <t>unit54 = Unit("54","61620","Otsego City","OtsegoCity","",Otsego City",Otsego",City")</t>
+  </si>
+  <si>
+    <t>unit55 = Unit("55","64740","Plainwell City","PlainwellCity","",Plainwell City",Plainwell",City")</t>
+  </si>
+  <si>
+    <t>unit56 = Unit("56","71700","Saugatuck City","SaugatuckCity","",Saugatuck City",Saugatuck",City")</t>
+  </si>
+  <si>
+    <t>unit57 = Unit("57","74980","South Haven City","South HavenCity","",South Haven City",South Haven",City")</t>
+  </si>
+  <si>
+    <t>unit58 = Unit("58","84880","Wayland City","WaylandCity","",Wayland City",Wayland",City")</t>
+  </si>
+  <si>
+    <t>unit59 = Unit("59","22740","Douglas City","DouglasCity","",Douglas City",Douglas",City")</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2703,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2132,12 +2711,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2153,6 +2827,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="UnitList" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="UnitList" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2418,10 +3100,1172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="120.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B1" t="str">
+        <f>CONCATENATE("unit"&amp;C1&amp;" = Unit("&amp;CHAR(34)&amp;C1&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;D1&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;E1&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;F1&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;G1&amp;CHAR(34)&amp;CHAR(34)&amp;","&amp;H1&amp;CHAR(34)&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;I1&amp;CHAR(34)&amp;","&amp;J1&amp;CHAR(34)&amp;")")</f>
+        <v>unit01 = Unit("01","01280","Allegan Twp","AlleganTwp","T2NR13W"",Allegan Township"","Allegan",Township")</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>809</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>837</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B35" si="0">CONCATENATE("unit"&amp;C2&amp;" = Unit("&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;F2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;G2&amp;CHAR(34)&amp;","&amp;H2&amp;CHAR(34)&amp;","&amp;I2&amp;CHAR(34)&amp;","&amp;J2&amp;CHAR(34)&amp;")")</f>
+        <v>unit02 = Unit("02","13700","Casco Twp","CascoTwp","T1NR16W",Casco Township",Casco",Township")</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="13">
+        <v>13700</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>838</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>unit03 = Unit("03","15200","Cheshire Twp","CheshireTwp","T1NR14W",Cheshire Township",Cheshire",Township")</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="13">
+        <v>15200</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>839</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>unit04 = Unit("04","16720","Clyde Twp","ClydeTwp","T2NR15W",Clyde Township",Clyde",Township")</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="13">
+        <v>16720</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>840</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>unit05 = Unit("05","22680","Dorr Twp","DorrTwp","T4NR12W",Dorr Township",Dorr",Township")</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="13">
+        <v>22680</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>841</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>unit06 = Unit("06","28120","Fillmore Twp","FillmoreTwp","T4NR15W",Fillmore Township",Fillmore",Township")</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="13">
+        <v>28120</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>842</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>unit07 = Unit("07","31360","Ganges Twp","GangesTwp","T2NR16W",Ganges Township",Ganges",Township")</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="13">
+        <v>31360</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>843</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>unit08 = Unit("08","35720","Gun Plain Twp","GunPlainTwp","T1NR11W",Gun Plain Township",Gun Plain",Township")</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="13">
+        <v>35720</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>844</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>unit09 = Unit("09","37460","Heath Twp","HeathTwp","T3NR14W",Heath Township",Heath",Township")</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="13">
+        <v>37460</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>845</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>unit10 = Unit("10","39200","Hopkins Twp","HopkinsTwp","T3NR12W",Hopkins Township",Hopkins",Township")</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="13">
+        <v>39200</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>846</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>unit11 = Unit("11","45180","Laketown Twp","LaketownTwp","T4NR16W",Laketown Township",Laketown",Township")</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="13">
+        <v>45180</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>847</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>unit12 = Unit("12","46600","Lee Twp","LeeTwp","T1NR15W",Lee Township",Lee",Township")</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="13">
+        <v>46600</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>823</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>848</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>unit13 = Unit("13","46760","Leighton Twp","LeightonTwp","T4NR11W",Leighton Township",Leighton",Township")</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="13">
+        <v>46760</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>849</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>unit14 = Unit("14","50840","Manlius Twp","ManliusTwp","T3NR15W",Manlius Township",Manlius",Township")</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="13">
+        <v>50840</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>850</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>unit15 = Unit("15","52000","Martin Twp","MartinTwp","T2NR11W",Martin Township",Martin",Township")</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="13">
+        <v>52000</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>851</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>unit16 = Unit("16","55200","Monterey Twp","MontereyTwp","T3NR13W",Monterey Township",Monterey",Township")</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="13">
+        <v>55200</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>852</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>unit17 = Unit("17","61640","Otsego Twp","OtsegoTwp","T1NR12W",Otsego Township",Otsego",Township")</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="13">
+        <v>61640</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>777</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>853</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>unit18 = Unit("18","61820","Overisel Twp","OveriselTwp","T4NR14W",Overisel Township",Overisel",Township")</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="13">
+        <v>61820</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>854</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>unit19 = Unit("19","71100","Salem Twp","SalemTwp","T4NR13W",Salem Township",Salem",Township")</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="13">
+        <v>71100</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>855</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>unit20 = Unit("20","71720","Saugatuck Twp","SaugatuckTwp","T3NR16W",Saugatuck Township",Saugatucl",Township")</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="13">
+        <v>71720</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>856</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>unit21 = Unit("21","80620","Trowbridge Twp","TrowbridgeTwp","T1NR13W",Trowbridge Township",Trowbridge",Township")</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="13">
+        <v>80620</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>857</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>unit22 = Unit("22","81580","Valley Twp","ValleyTwp","T2NR14W",Valley Township",Valley",Township")</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="13">
+        <v>81580</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>858</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>unit23 = Unit("23","84580","Watson Twp","WatsonTwp","T2NR12W",Watson Township",Watson",Township")</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="13">
+        <v>84580</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>859</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>unit24 = Unit("24","84900","Wayland Twp","WaylandTwp","T3NR11W",Wayland Township",Wayland",Township")</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="13">
+        <v>84900</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>860</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>unit42 = Unit("42","39200","Hopkins Village","Hopkins Village","",Hopkins Village",Hopkins",Village")</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="13">
+        <v>39200</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>861</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>unit44 = Unit("44","52000","Martin Village","Martin Village","",Martin Village",Martin",Village")</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="13">
+        <v>52000</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>862</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>unit51 = Unit("51","01260","Allegan City","AlleganCity","",Allegan City",Allegan",City")</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>808</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>863</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>unit52 = Unit("52","27740","Fennville City","FennvilleCity","",Fennville City",Fennville",City")</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="13">
+        <v>27740</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>864</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>unit53 = Unit("53","38640","Holland City","HollandCity","",Holland City",Holland",City")</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>810</v>
+      </c>
+      <c r="D29" s="13">
+        <v>38640</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>865</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>unit54 = Unit("54","61620","Otsego City","OtsegoCity","",Otsego City",Otsego",City")</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="13">
+        <v>61620</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>866</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>unit55 = Unit("55","64740","Plainwell City","PlainwellCity","",Plainwell City",Plainwell",City")</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="13">
+        <v>64740</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>867</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>unit56 = Unit("56","71700","Saugatuck City","SaugatuckCity","",Saugatuck City",Saugatuck",City")</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="13">
+        <v>71700</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>868</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>unit57 = Unit("57","74980","South Haven City","South HavenCity","",South Haven City",South Haven",City")</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="13">
+        <v>74980</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>869</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>unit58 = Unit("58","84880","Wayland City","WaylandCity","",Wayland City",Wayland",City")</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>811</v>
+      </c>
+      <c r="D34" s="13">
+        <v>84880</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>870</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>unit59 = Unit("59","22740","Douglas City","DouglasCity","",Douglas City",Douglas",City")</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="15">
+        <v>22740</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>697</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C1:C35" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13528,7 +15372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M264"/>
   <sheetViews>
@@ -13593,7 +15437,7 @@
         <v>151</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="A2:B33" si="0">CONCATENATE(C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2)</f>
+        <f t="shared" ref="B2:B33" si="0">CONCATENATE(C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2)</f>
         <v xml:space="preserve">copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.shp J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.shp </v>
       </c>
       <c r="C2" t="s">
@@ -14979,7 +16823,7 @@
         <v>190</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" ref="A35:B66" si="1">CONCATENATE(C35&amp;D35&amp;E35&amp;F35&amp;G35&amp;H35&amp;I35&amp;J35&amp;K35&amp;L35&amp;M35)</f>
+        <f t="shared" ref="B35:B66" si="1">CONCATENATE(C35&amp;D35&amp;E35&amp;F35&amp;G35&amp;H35&amp;I35&amp;J35&amp;K35&amp;L35&amp;M35)</f>
         <v>copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.dbf J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.dbf</v>
       </c>
       <c r="C35" t="s">
@@ -16365,7 +18209,7 @@
         <v>223</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" ref="A68:B99" si="2">CONCATENATE(C68&amp;D68&amp;E68&amp;F68&amp;G68&amp;H68&amp;I68&amp;J68&amp;K68&amp;L68&amp;M68)</f>
+        <f t="shared" ref="B68:B99" si="2">CONCATENATE(C68&amp;D68&amp;E68&amp;F68&amp;G68&amp;H68&amp;I68&amp;J68&amp;K68&amp;L68&amp;M68)</f>
         <v>copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.shx J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.shx</v>
       </c>
       <c r="C68" t="s">
@@ -17751,7 +19595,7 @@
         <v>256</v>
       </c>
       <c r="B101" t="str">
-        <f t="shared" ref="A101:B132" si="3">CONCATENATE(C101&amp;D101&amp;E101&amp;F101&amp;G101&amp;H101&amp;I101&amp;J101&amp;K101&amp;L101&amp;M101)</f>
+        <f t="shared" ref="B101:B132" si="3">CONCATENATE(C101&amp;D101&amp;E101&amp;F101&amp;G101&amp;H101&amp;I101&amp;J101&amp;K101&amp;L101&amp;M101)</f>
         <v>copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.prj J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.prj</v>
       </c>
       <c r="C101" t="s">
@@ -19137,7 +20981,7 @@
         <v>289</v>
       </c>
       <c r="B134" t="str">
-        <f t="shared" ref="A134:B165" si="4">CONCATENATE(C134&amp;D134&amp;E134&amp;F134&amp;G134&amp;H134&amp;I134&amp;J134&amp;K134&amp;L134&amp;M134)</f>
+        <f t="shared" ref="B134:B165" si="4">CONCATENATE(C134&amp;D134&amp;E134&amp;F134&amp;G134&amp;H134&amp;I134&amp;J134&amp;K134&amp;L134&amp;M134)</f>
         <v xml:space="preserve">copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.cpg J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.cpg </v>
       </c>
       <c r="C134" t="s">
@@ -20523,7 +22367,7 @@
         <v>322</v>
       </c>
       <c r="B167" t="str">
-        <f t="shared" ref="A167:B198" si="5">CONCATENATE(C167&amp;D167&amp;E167&amp;F167&amp;G167&amp;H167&amp;I167&amp;J167&amp;K167&amp;L167&amp;M167)</f>
+        <f t="shared" ref="B167:B198" si="5">CONCATENATE(C167&amp;D167&amp;E167&amp;F167&amp;G167&amp;H167&amp;I167&amp;J167&amp;K167&amp;L167&amp;M167)</f>
         <v xml:space="preserve">copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.sbn J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.sbn </v>
       </c>
       <c r="C167" t="s">
@@ -21909,7 +23753,7 @@
         <v>358</v>
       </c>
       <c r="B200" t="str">
-        <f t="shared" ref="A200:B231" si="6">CONCATENATE(C200&amp;D200&amp;E200&amp;F200&amp;G200&amp;H200&amp;I200&amp;J200&amp;K200&amp;L200&amp;M200)</f>
+        <f t="shared" ref="B200:B231" si="6">CONCATENATE(C200&amp;D200&amp;E200&amp;F200&amp;G200&amp;H200&amp;I200&amp;J200&amp;K200&amp;L200&amp;M200)</f>
         <v>copy J:\Apps\Products\AccuGlobe\LocalUnits\build\02CascoTwp\IntlFt\Parcels.shp.xml J:\data\Shapefiles\02CascoTwp\IntlFt\Parcels.shp.xml</v>
       </c>
       <c r="C200" t="s">
@@ -24639,7 +26483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -24654,7 +26498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
@@ -25568,7 +27412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
@@ -26484,7 +28328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
@@ -27198,7 +29042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
@@ -27912,12 +29756,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E35" sqref="E1:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27925,369 +29769,1298 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>809</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="2">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="13">
+        <v>13700</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="13">
+        <v>15200</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="5">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="13">
+        <v>16720</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="5">
+        <v>4</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="13">
+        <v>22680</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="5">
+        <v>5</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="13">
+        <v>28120</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="5">
+        <v>6</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="13">
+        <v>31360</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="5">
+        <v>7</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="13">
+        <v>35720</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="5">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="13">
+        <v>37460</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="5">
+        <v>9</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="13">
+        <v>39200</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="5">
+        <v>10</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="13">
+        <v>45180</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="5">
+        <v>11</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="13">
+        <v>46600</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="5">
+        <v>12</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E13" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="13">
+        <v>46760</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="5">
+        <v>13</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="13">
+        <v>50840</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="5">
+        <v>14</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="13">
+        <v>52000</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="5">
+        <v>15</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="13">
+        <v>55200</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="5">
+        <v>16</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="13">
+        <v>61640</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="5">
+        <v>17</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>777</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E18" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="13">
+        <v>61820</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="5">
+        <v>18</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E19" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="13">
+        <v>71100</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="5">
+        <v>19</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="13">
+        <v>71720</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="5">
+        <v>20</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="13">
+        <v>80620</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="5">
+        <v>21</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="E22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="13">
+        <v>81580</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="5">
+        <v>22</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="E23" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="13">
+        <v>84580</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="5">
+        <v>23</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="E24" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="13">
+        <v>84900</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="5">
+        <v>24</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="E25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="13">
+        <v>39200</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="I25" s="5">
+        <v>44</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="E26" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="13">
+        <v>52000</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="I26" s="5">
+        <v>42</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="E27" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>808</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" s="5">
+        <v>51</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="E28" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="13">
+        <v>27740</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="5">
+        <v>52</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="E29" s="12" t="s">
+        <v>810</v>
+      </c>
+      <c r="F29" s="13">
+        <v>38640</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="I29" s="5">
+        <v>53</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="E30" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="13">
+        <v>61620</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="5">
+        <v>54</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E31" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="13">
+        <v>64740</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="5">
+        <v>55</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="E32" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="13">
+        <v>71700</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="5">
+        <v>57</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="9" t="s">
         <v>67</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="13">
+        <v>74980</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="I33" s="5">
+        <v>58</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="12" t="s">
+        <v>811</v>
+      </c>
+      <c r="F34" s="13">
+        <v>84880</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="5">
+        <v>56</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="15">
+        <v>22740</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="8">
+        <v>59</v>
+      </c>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transposed unit list
</commit_message>
<xml_diff>
--- a/processing/commands.xlsx
+++ b/processing/commands.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="6345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="6345" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="pyclassUnit" sheetId="11" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="make_directory_in_S" sheetId="9" r:id="rId7"/>
     <sheet name="make_directory" sheetId="3" r:id="rId8"/>
     <sheet name="lists" sheetId="2" r:id="rId9"/>
+    <sheet name="lists_transposed" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="UnitList" localSheetId="8">lists!$F$1:$M$34</definedName>
+    <definedName name="UnitList" localSheetId="8">lists!$H$1:$O$34</definedName>
     <definedName name="UnitList" localSheetId="0">pyclassUnit!$D$1:$J$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -63,11 +64,76 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="UnitList12" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="UnitList13" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="UnitList14" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="UnitList15" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="UnitList16" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\apps\python\ESRI\Translate\processing\UnitList.txt" tab="0" comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7768" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8082" uniqueCount="949">
   <si>
     <t>01AlleganTwp</t>
   </si>
@@ -2680,6 +2746,240 @@
   </si>
   <si>
     <t>"unit59",</t>
+  </si>
+  <si>
+    <t>unit01</t>
+  </si>
+  <si>
+    <t>unit02</t>
+  </si>
+  <si>
+    <t>unit03</t>
+  </si>
+  <si>
+    <t>unit04</t>
+  </si>
+  <si>
+    <t>unit05</t>
+  </si>
+  <si>
+    <t>unit06</t>
+  </si>
+  <si>
+    <t>unit07</t>
+  </si>
+  <si>
+    <t>unit08</t>
+  </si>
+  <si>
+    <t>unit09</t>
+  </si>
+  <si>
+    <t>unit10</t>
+  </si>
+  <si>
+    <t>unit11</t>
+  </si>
+  <si>
+    <t>unit12</t>
+  </si>
+  <si>
+    <t>unit13</t>
+  </si>
+  <si>
+    <t>unit14</t>
+  </si>
+  <si>
+    <t>unit15</t>
+  </si>
+  <si>
+    <t>unit16</t>
+  </si>
+  <si>
+    <t>unit17</t>
+  </si>
+  <si>
+    <t>unit18</t>
+  </si>
+  <si>
+    <t>unit19</t>
+  </si>
+  <si>
+    <t>unit20</t>
+  </si>
+  <si>
+    <t>unit21</t>
+  </si>
+  <si>
+    <t>unit22</t>
+  </si>
+  <si>
+    <t>unit23</t>
+  </si>
+  <si>
+    <t>unit24</t>
+  </si>
+  <si>
+    <t>unit44</t>
+  </si>
+  <si>
+    <t>unit42</t>
+  </si>
+  <si>
+    <t>unit51</t>
+  </si>
+  <si>
+    <t>unit52</t>
+  </si>
+  <si>
+    <t>unit53</t>
+  </si>
+  <si>
+    <t>unit54</t>
+  </si>
+  <si>
+    <t>unit55</t>
+  </si>
+  <si>
+    <t>unit56</t>
+  </si>
+  <si>
+    <t>unit57</t>
+  </si>
+  <si>
+    <t>unit58</t>
+  </si>
+  <si>
+    <t>unit59</t>
+  </si>
+  <si>
+    <t>unit01,unit02,unit03,unit04,unit05,unit06,unit07,unit08,unit09,unit10,unit11,unit12,unit13,unit14,unit15,unit16,unit17,unit18,unit19,unit20,unit21,unit22,unit23,unit24,unit42,unit44,unit51,unit52,unit53,unit54,unit55,unit56,unit57,unit58,unit59</t>
+  </si>
+  <si>
+    <t>01,02,03,04,05,06,07,08,09,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,42,44,51,52,53,54,55,56,57,58,59</t>
+  </si>
+  <si>
+    <t>01280,13700,15200,16720,22680,28120,31360,35720,37460,39200,45180,46600,46760,50840,52000,55200,61640,61820,71100,71720,80620,81580,84580,84900,39200,52000,01260,27740,38640,61620,64740,71700,74980,84880,22740</t>
+  </si>
+  <si>
+    <t>Allegan Twp,Casco Twp,Cheshire Twp,Clyde Twp,Dorr Twp,Fillmore Twp,Ganges Twp,Gun Plain Twp,Heath Twp,Hopkins Twp,Laketown Twp,Lee Twp,Leighton Twp,Manlius Twp,Martin Twp,Monterey Twp,Otsego Twp,Overisel Twp,Salem Twp,Saugatuck Twp,Trowbridge Twp,Valley Twp,Watson Twp,Wayland Twp,Hopkins Village,Martin Village,Allegan City,Fennville City,Holland City,Otsego City,Plainwell City,Saugatuck City,South Haven City,Wayland City,Douglas City</t>
+  </si>
+  <si>
+    <t>AlleganTwp,CascoTwp,CheshireTwp,ClydeTwp,DorrTwp,FillmoreTwp,GangesTwp,GunPlainTwp,HeathTwp,HopkinsTwp,LaketownTwp,LeeTwp,LeightonTwp,ManliusTwp,MartinTwp,MontereyTwp,OtsegoTwp,OveriselTwp,SalemTwp,SaugatuckTwp,TrowbridgeTwp,ValleyTwp,WatsonTwp,WaylandTwp,Hopkins Village,Martin Village,AlleganCity,FennvilleCity,HollandCity,OtsegoCity,PlainwellCity,SaugatuckCity,South HavenCity,WaylandCity,DouglasCity</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,44,42,51,52,53,54,55,57,58,56,59</t>
+  </si>
+  <si>
+    <t>T2N  R13W,T1N  R16W,T1N  R14W,T2N  R15W,T4N  R12W,T4N  R15W,T2N  R16W,T1N  R11W,T3N  R14W,T3N  R12W,T4N  R16W,T1N  R15W,T4N  R11W,T3N  R15W,T2N  R11W,T3N  R13W,T1N  R12W,T4N  R14W,T4N  R13W,T3N  R16W,T1N  R13W,T2N  R14W,T2N  R12W,T3N  R11W,,,,,,,,,,,</t>
+  </si>
+  <si>
+    <t>Allegan Township,Casco Township,Cheshire Township,Clyde Township,Dorr Township,Fillmore Township,Ganges Township,Gun Plain Township,Heath Township,Hopkins Township,Laketown Township,Lee Township,Leighton Township,Manlius Township,Martin Township,Monterey Township,Otsego Township,Overisel Township,Salem Township,Saugatuck Township,Trowbridge Township,Valley Township,Watson Township,Wayland Township,Hopkins Village,Martin Village,Allegan City,Fennville City,Holland City,Otsego City,Plainwell City,Saugatuck City,South Haven City,Wayland City,Douglas City</t>
+  </si>
+  <si>
+    <t>Allegan,Casco,Cheshire,Clyde,Dorr,Fillmore,Ganges,Gun Plain,Heath,Hopkins,Laketown,Lee,Leighton,Manlius,Martin,Monterey,Otsego,Overisel,Salem,Saugatucl,Trowbridge,Valley,Watson,Wayland,Hopkins,Martin,Allegan,Fennville,Holland,Otsego,Plainwell,Saugatuck,South Haven,Wayland,Douglas</t>
+  </si>
+  <si>
+    <t>Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Village,Village,City,City,City,City,City,City,City,City,City</t>
+  </si>
+  <si>
+    <t>self.unit01 = unit01</t>
+  </si>
+  <si>
+    <t>self.unit02 = unit02</t>
+  </si>
+  <si>
+    <t>self.unit03 = unit03</t>
+  </si>
+  <si>
+    <t>self.unit04 = unit04</t>
+  </si>
+  <si>
+    <t>self.unit05 = unit05</t>
+  </si>
+  <si>
+    <t>self.unit06 = unit06</t>
+  </si>
+  <si>
+    <t>self.unit07 = unit07</t>
+  </si>
+  <si>
+    <t>self.unit08 = unit08</t>
+  </si>
+  <si>
+    <t>self.unit09 = unit09</t>
+  </si>
+  <si>
+    <t>self.unit10 = unit10</t>
+  </si>
+  <si>
+    <t>self.unit11 = unit11</t>
+  </si>
+  <si>
+    <t>self.unit12 = unit12</t>
+  </si>
+  <si>
+    <t>self.unit13 = unit13</t>
+  </si>
+  <si>
+    <t>self.unit14 = unit14</t>
+  </si>
+  <si>
+    <t>self.unit15 = unit15</t>
+  </si>
+  <si>
+    <t>self.unit16 = unit16</t>
+  </si>
+  <si>
+    <t>self.unit17 = unit17</t>
+  </si>
+  <si>
+    <t>self.unit18 = unit18</t>
+  </si>
+  <si>
+    <t>self.unit19 = unit19</t>
+  </si>
+  <si>
+    <t>self.unit20 = unit20</t>
+  </si>
+  <si>
+    <t>self.unit21 = unit21</t>
+  </si>
+  <si>
+    <t>self.unit22 = unit22</t>
+  </si>
+  <si>
+    <t>self.unit23 = unit23</t>
+  </si>
+  <si>
+    <t>self.unit24 = unit24</t>
+  </si>
+  <si>
+    <t>self.unit42 = unit42</t>
+  </si>
+  <si>
+    <t>self.unit44 = unit44</t>
+  </si>
+  <si>
+    <t>self.unit51 = unit51</t>
+  </si>
+  <si>
+    <t>self.unit52 = unit52</t>
+  </si>
+  <si>
+    <t>self.unit53 = unit53</t>
+  </si>
+  <si>
+    <t>self.unit54 = unit54</t>
+  </si>
+  <si>
+    <t>self.unit55 = unit55</t>
+  </si>
+  <si>
+    <t>self.unit56 = unit56</t>
+  </si>
+  <si>
+    <t>self.unit57 = unit57</t>
   </si>
 </sst>
 </file>
@@ -3102,7 +3402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:A35"/>
     </sheetView>
   </sheetViews>
@@ -4572,6 +4872,1171 @@
   <ignoredErrors>
     <ignoredError sqref="C1:C35" numberStoredAsText="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C1" t="s">
+        <v>873</v>
+      </c>
+      <c r="D1" t="s">
+        <v>874</v>
+      </c>
+      <c r="E1" t="s">
+        <v>875</v>
+      </c>
+      <c r="F1" t="s">
+        <v>876</v>
+      </c>
+      <c r="G1" t="s">
+        <v>877</v>
+      </c>
+      <c r="H1" t="s">
+        <v>878</v>
+      </c>
+      <c r="I1" t="s">
+        <v>879</v>
+      </c>
+      <c r="J1" t="s">
+        <v>880</v>
+      </c>
+      <c r="K1" t="s">
+        <v>881</v>
+      </c>
+      <c r="L1" t="s">
+        <v>882</v>
+      </c>
+      <c r="M1" t="s">
+        <v>883</v>
+      </c>
+      <c r="N1" t="s">
+        <v>884</v>
+      </c>
+      <c r="O1" t="s">
+        <v>885</v>
+      </c>
+      <c r="P1" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>887</v>
+      </c>
+      <c r="R1" t="s">
+        <v>888</v>
+      </c>
+      <c r="S1" t="s">
+        <v>889</v>
+      </c>
+      <c r="T1" t="s">
+        <v>890</v>
+      </c>
+      <c r="U1" t="s">
+        <v>891</v>
+      </c>
+      <c r="V1" t="s">
+        <v>892</v>
+      </c>
+      <c r="W1" t="s">
+        <v>893</v>
+      </c>
+      <c r="X1" t="s">
+        <v>894</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>896</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>895</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>897</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>898</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>899</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>900</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>901</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>902</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>903</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>904</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>810</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>811</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>809</v>
+      </c>
+      <c r="B3">
+        <v>13700</v>
+      </c>
+      <c r="C3">
+        <v>15200</v>
+      </c>
+      <c r="D3">
+        <v>16720</v>
+      </c>
+      <c r="E3">
+        <v>22680</v>
+      </c>
+      <c r="F3">
+        <v>28120</v>
+      </c>
+      <c r="G3">
+        <v>31360</v>
+      </c>
+      <c r="H3">
+        <v>35720</v>
+      </c>
+      <c r="I3">
+        <v>37460</v>
+      </c>
+      <c r="J3">
+        <v>39200</v>
+      </c>
+      <c r="K3">
+        <v>45180</v>
+      </c>
+      <c r="L3">
+        <v>46600</v>
+      </c>
+      <c r="M3">
+        <v>46760</v>
+      </c>
+      <c r="N3">
+        <v>50840</v>
+      </c>
+      <c r="O3">
+        <v>52000</v>
+      </c>
+      <c r="P3">
+        <v>55200</v>
+      </c>
+      <c r="Q3">
+        <v>61640</v>
+      </c>
+      <c r="R3">
+        <v>61820</v>
+      </c>
+      <c r="S3">
+        <v>71100</v>
+      </c>
+      <c r="T3">
+        <v>71720</v>
+      </c>
+      <c r="U3">
+        <v>80620</v>
+      </c>
+      <c r="V3">
+        <v>81580</v>
+      </c>
+      <c r="W3">
+        <v>84580</v>
+      </c>
+      <c r="X3">
+        <v>84900</v>
+      </c>
+      <c r="Y3">
+        <v>39200</v>
+      </c>
+      <c r="Z3">
+        <v>52000</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>808</v>
+      </c>
+      <c r="AB3">
+        <v>27740</v>
+      </c>
+      <c r="AC3">
+        <v>38640</v>
+      </c>
+      <c r="AD3">
+        <v>61620</v>
+      </c>
+      <c r="AE3">
+        <v>64740</v>
+      </c>
+      <c r="AF3">
+        <v>71700</v>
+      </c>
+      <c r="AG3">
+        <v>74980</v>
+      </c>
+      <c r="AH3">
+        <v>84880</v>
+      </c>
+      <c r="AI3">
+        <v>22740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4" t="s">
+        <v>790</v>
+      </c>
+      <c r="C4" t="s">
+        <v>735</v>
+      </c>
+      <c r="D4" t="s">
+        <v>769</v>
+      </c>
+      <c r="E4" t="s">
+        <v>723</v>
+      </c>
+      <c r="F4" t="s">
+        <v>794</v>
+      </c>
+      <c r="G4" t="s">
+        <v>784</v>
+      </c>
+      <c r="H4" t="s">
+        <v>698</v>
+      </c>
+      <c r="I4" t="s">
+        <v>706</v>
+      </c>
+      <c r="J4" t="s">
+        <v>751</v>
+      </c>
+      <c r="K4" t="s">
+        <v>778</v>
+      </c>
+      <c r="L4" t="s">
+        <v>739</v>
+      </c>
+      <c r="M4" t="s">
+        <v>759</v>
+      </c>
+      <c r="N4" t="s">
+        <v>765</v>
+      </c>
+      <c r="O4" t="s">
+        <v>746</v>
+      </c>
+      <c r="P4" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>775</v>
+      </c>
+      <c r="R4" t="s">
+        <v>727</v>
+      </c>
+      <c r="S4" t="s">
+        <v>702</v>
+      </c>
+      <c r="T4" t="s">
+        <v>798</v>
+      </c>
+      <c r="U4" t="s">
+        <v>715</v>
+      </c>
+      <c r="V4" t="s">
+        <v>731</v>
+      </c>
+      <c r="W4" t="s">
+        <v>719</v>
+      </c>
+      <c r="X4" t="s">
+        <v>756</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>749</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>743</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>710</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>763</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>804</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>695</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>773</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>802</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>788</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>754</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" t="s">
+        <v>57</v>
+      </c>
+      <c r="X5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>749</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>743</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>807</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>806</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>13</v>
+      </c>
+      <c r="N6">
+        <v>14</v>
+      </c>
+      <c r="O6">
+        <v>15</v>
+      </c>
+      <c r="P6">
+        <v>16</v>
+      </c>
+      <c r="Q6">
+        <v>17</v>
+      </c>
+      <c r="R6">
+        <v>18</v>
+      </c>
+      <c r="S6">
+        <v>19</v>
+      </c>
+      <c r="T6">
+        <v>20</v>
+      </c>
+      <c r="U6">
+        <v>21</v>
+      </c>
+      <c r="V6">
+        <v>22</v>
+      </c>
+      <c r="W6">
+        <v>23</v>
+      </c>
+      <c r="X6">
+        <v>24</v>
+      </c>
+      <c r="Y6">
+        <v>44</v>
+      </c>
+      <c r="Z6">
+        <v>42</v>
+      </c>
+      <c r="AA6">
+        <v>51</v>
+      </c>
+      <c r="AB6">
+        <v>52</v>
+      </c>
+      <c r="AC6">
+        <v>53</v>
+      </c>
+      <c r="AD6">
+        <v>54</v>
+      </c>
+      <c r="AE6">
+        <v>55</v>
+      </c>
+      <c r="AF6">
+        <v>57</v>
+      </c>
+      <c r="AG6">
+        <v>58</v>
+      </c>
+      <c r="AH6">
+        <v>56</v>
+      </c>
+      <c r="AI6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>713</v>
+      </c>
+      <c r="B7" t="s">
+        <v>791</v>
+      </c>
+      <c r="C7" t="s">
+        <v>736</v>
+      </c>
+      <c r="D7" t="s">
+        <v>770</v>
+      </c>
+      <c r="E7" t="s">
+        <v>724</v>
+      </c>
+      <c r="F7" t="s">
+        <v>795</v>
+      </c>
+      <c r="G7" t="s">
+        <v>785</v>
+      </c>
+      <c r="H7" t="s">
+        <v>699</v>
+      </c>
+      <c r="I7" t="s">
+        <v>707</v>
+      </c>
+      <c r="J7" t="s">
+        <v>752</v>
+      </c>
+      <c r="K7" t="s">
+        <v>779</v>
+      </c>
+      <c r="L7" t="s">
+        <v>740</v>
+      </c>
+      <c r="M7" t="s">
+        <v>760</v>
+      </c>
+      <c r="N7" t="s">
+        <v>766</v>
+      </c>
+      <c r="O7" t="s">
+        <v>747</v>
+      </c>
+      <c r="P7" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>776</v>
+      </c>
+      <c r="R7" t="s">
+        <v>728</v>
+      </c>
+      <c r="S7" t="s">
+        <v>703</v>
+      </c>
+      <c r="T7" t="s">
+        <v>799</v>
+      </c>
+      <c r="U7" t="s">
+        <v>716</v>
+      </c>
+      <c r="V7" t="s">
+        <v>732</v>
+      </c>
+      <c r="W7" t="s">
+        <v>720</v>
+      </c>
+      <c r="X7" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>714</v>
+      </c>
+      <c r="B8" t="s">
+        <v>792</v>
+      </c>
+      <c r="C8" t="s">
+        <v>737</v>
+      </c>
+      <c r="D8" t="s">
+        <v>771</v>
+      </c>
+      <c r="E8" t="s">
+        <v>725</v>
+      </c>
+      <c r="F8" t="s">
+        <v>796</v>
+      </c>
+      <c r="G8" t="s">
+        <v>786</v>
+      </c>
+      <c r="H8" t="s">
+        <v>700</v>
+      </c>
+      <c r="I8" t="s">
+        <v>708</v>
+      </c>
+      <c r="J8" t="s">
+        <v>753</v>
+      </c>
+      <c r="K8" t="s">
+        <v>780</v>
+      </c>
+      <c r="L8" t="s">
+        <v>741</v>
+      </c>
+      <c r="M8" t="s">
+        <v>761</v>
+      </c>
+      <c r="N8" t="s">
+        <v>767</v>
+      </c>
+      <c r="O8" t="s">
+        <v>748</v>
+      </c>
+      <c r="P8" t="s">
+        <v>692</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>777</v>
+      </c>
+      <c r="R8" t="s">
+        <v>729</v>
+      </c>
+      <c r="S8" t="s">
+        <v>704</v>
+      </c>
+      <c r="T8" t="s">
+        <v>800</v>
+      </c>
+      <c r="U8" t="s">
+        <v>717</v>
+      </c>
+      <c r="V8" t="s">
+        <v>733</v>
+      </c>
+      <c r="W8" t="s">
+        <v>721</v>
+      </c>
+      <c r="X8" t="s">
+        <v>758</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>749</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>743</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>710</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>763</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>804</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>695</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>773</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>802</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>788</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>754</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>711</v>
+      </c>
+      <c r="B9" t="s">
+        <v>793</v>
+      </c>
+      <c r="C9" t="s">
+        <v>738</v>
+      </c>
+      <c r="D9" t="s">
+        <v>772</v>
+      </c>
+      <c r="E9" t="s">
+        <v>726</v>
+      </c>
+      <c r="F9" t="s">
+        <v>797</v>
+      </c>
+      <c r="G9" t="s">
+        <v>787</v>
+      </c>
+      <c r="H9" t="s">
+        <v>701</v>
+      </c>
+      <c r="I9" t="s">
+        <v>709</v>
+      </c>
+      <c r="J9" t="s">
+        <v>750</v>
+      </c>
+      <c r="K9" t="s">
+        <v>781</v>
+      </c>
+      <c r="L9" t="s">
+        <v>742</v>
+      </c>
+      <c r="M9" t="s">
+        <v>762</v>
+      </c>
+      <c r="N9" t="s">
+        <v>768</v>
+      </c>
+      <c r="O9" t="s">
+        <v>744</v>
+      </c>
+      <c r="P9" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>696</v>
+      </c>
+      <c r="R9" t="s">
+        <v>730</v>
+      </c>
+      <c r="S9" t="s">
+        <v>705</v>
+      </c>
+      <c r="T9" t="s">
+        <v>801</v>
+      </c>
+      <c r="U9" t="s">
+        <v>718</v>
+      </c>
+      <c r="V9" t="s">
+        <v>734</v>
+      </c>
+      <c r="W9" t="s">
+        <v>722</v>
+      </c>
+      <c r="X9" t="s">
+        <v>755</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>750</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>744</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>711</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>764</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>805</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>696</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>774</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>803</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>789</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>755</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>694</v>
+      </c>
+      <c r="B10" t="s">
+        <v>694</v>
+      </c>
+      <c r="C10" t="s">
+        <v>694</v>
+      </c>
+      <c r="D10" t="s">
+        <v>694</v>
+      </c>
+      <c r="E10" t="s">
+        <v>694</v>
+      </c>
+      <c r="F10" t="s">
+        <v>694</v>
+      </c>
+      <c r="G10" t="s">
+        <v>694</v>
+      </c>
+      <c r="H10" t="s">
+        <v>694</v>
+      </c>
+      <c r="I10" t="s">
+        <v>694</v>
+      </c>
+      <c r="J10" t="s">
+        <v>694</v>
+      </c>
+      <c r="K10" t="s">
+        <v>694</v>
+      </c>
+      <c r="L10" t="s">
+        <v>694</v>
+      </c>
+      <c r="M10" t="s">
+        <v>694</v>
+      </c>
+      <c r="N10" t="s">
+        <v>694</v>
+      </c>
+      <c r="O10" t="s">
+        <v>694</v>
+      </c>
+      <c r="P10" t="s">
+        <v>694</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>694</v>
+      </c>
+      <c r="R10" t="s">
+        <v>694</v>
+      </c>
+      <c r="S10" t="s">
+        <v>694</v>
+      </c>
+      <c r="T10" t="s">
+        <v>694</v>
+      </c>
+      <c r="U10" t="s">
+        <v>694</v>
+      </c>
+      <c r="V10" t="s">
+        <v>694</v>
+      </c>
+      <c r="W10" t="s">
+        <v>694</v>
+      </c>
+      <c r="X10" t="s">
+        <v>694</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>745</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>745</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>697</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>CONCATENATE(A1&amp;","&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;","&amp;E1&amp;","&amp;F1&amp;","&amp;G1&amp;","&amp;H1&amp;","&amp;I1&amp;","&amp;J1&amp;","&amp;K1&amp;","&amp;L1&amp;","&amp;M1&amp;","&amp;N1&amp;","&amp;O1&amp;","&amp;P1&amp;","&amp;Q1&amp;","&amp;R1&amp;","&amp;S1&amp;","&amp;T1&amp;","&amp;U1&amp;","&amp;V1&amp;","&amp;W1&amp;","&amp;X1&amp;","&amp;Y1&amp;","&amp;Z1&amp;","&amp;AA1&amp;","&amp;AB1&amp;","&amp;AC1&amp;","&amp;AD1&amp;","&amp;AE1&amp;","&amp;AF1&amp;","&amp;AG1&amp;","&amp;AH1&amp;","&amp;AI1)</f>
+        <v>unit01,unit02,unit03,unit04,unit05,unit06,unit07,unit08,unit09,unit10,unit11,unit12,unit13,unit14,unit15,unit16,unit17,unit18,unit19,unit20,unit21,unit22,unit23,unit24,unit42,unit44,unit51,unit52,unit53,unit54,unit55,unit56,unit57,unit58,unit59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>CONCATENATE(A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;","&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;","&amp;M2&amp;","&amp;N2&amp;","&amp;O2&amp;","&amp;P2&amp;","&amp;Q2&amp;","&amp;R2&amp;","&amp;S2&amp;","&amp;T2&amp;","&amp;U2&amp;","&amp;V2&amp;","&amp;W2&amp;","&amp;X2&amp;","&amp;Y2&amp;","&amp;Z2&amp;","&amp;AA2&amp;","&amp;AB2&amp;","&amp;AC2&amp;","&amp;AD2&amp;","&amp;AE2&amp;","&amp;AF2&amp;","&amp;AG2&amp;","&amp;AH2&amp;","&amp;AI2)</f>
+        <v>01,02,03,04,05,06,07,08,09,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,42,44,51,52,53,54,55,56,57,58,59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>CONCATENATE(A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;U3&amp;","&amp;V3&amp;","&amp;W3&amp;","&amp;X3&amp;","&amp;Y3&amp;","&amp;Z3&amp;","&amp;AA3&amp;","&amp;AB3&amp;","&amp;AC3&amp;","&amp;AD3&amp;","&amp;AE3&amp;","&amp;AF3&amp;","&amp;AG3&amp;","&amp;AH3&amp;","&amp;AI3)</f>
+        <v>01280,13700,15200,16720,22680,28120,31360,35720,37460,39200,45180,46600,46760,50840,52000,55200,61640,61820,71100,71720,80620,81580,84580,84900,39200,52000,01260,27740,38640,61620,64740,71700,74980,84880,22740</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>CONCATENATE(A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4&amp;","&amp;J4&amp;","&amp;K4&amp;","&amp;L4&amp;","&amp;M4&amp;","&amp;N4&amp;","&amp;O4&amp;","&amp;P4&amp;","&amp;Q4&amp;","&amp;R4&amp;","&amp;S4&amp;","&amp;T4&amp;","&amp;U4&amp;","&amp;V4&amp;","&amp;W4&amp;","&amp;X4&amp;","&amp;Y4&amp;","&amp;Z4&amp;","&amp;AA4&amp;","&amp;AB4&amp;","&amp;AC4&amp;","&amp;AD4&amp;","&amp;AE4&amp;","&amp;AF4&amp;","&amp;AG4&amp;","&amp;AH4&amp;","&amp;AI4)</f>
+        <v>Allegan Twp,Casco Twp,Cheshire Twp,Clyde Twp,Dorr Twp,Fillmore Twp,Ganges Twp,Gun Plain Twp,Heath Twp,Hopkins Twp,Laketown Twp,Lee Twp,Leighton Twp,Manlius Twp,Martin Twp,Monterey Twp,Otsego Twp,Overisel Twp,Salem Twp,Saugatuck Twp,Trowbridge Twp,Valley Twp,Watson Twp,Wayland Twp,Hopkins Village,Martin Village,Allegan City,Fennville City,Holland City,Otsego City,Plainwell City,Saugatuck City,South Haven City,Wayland City,Douglas City</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>CONCATENATE(A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;K5&amp;","&amp;L5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;O5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;S5&amp;","&amp;T5&amp;","&amp;U5&amp;","&amp;V5&amp;","&amp;W5&amp;","&amp;X5&amp;","&amp;Y5&amp;","&amp;Z5&amp;","&amp;AA5&amp;","&amp;AB5&amp;","&amp;AC5&amp;","&amp;AD5&amp;","&amp;AE5&amp;","&amp;AF5&amp;","&amp;AG5&amp;","&amp;AH5&amp;","&amp;AI5)</f>
+        <v>AlleganTwp,CascoTwp,CheshireTwp,ClydeTwp,DorrTwp,FillmoreTwp,GangesTwp,GunPlainTwp,HeathTwp,HopkinsTwp,LaketownTwp,LeeTwp,LeightonTwp,ManliusTwp,MartinTwp,MontereyTwp,OtsegoTwp,OveriselTwp,SalemTwp,SaugatuckTwp,TrowbridgeTwp,ValleyTwp,WatsonTwp,WaylandTwp,Hopkins Village,Martin Village,AlleganCity,FennvilleCity,HollandCity,OtsegoCity,PlainwellCity,SaugatuckCity,South HavenCity,WaylandCity,DouglasCity</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>CONCATENATE(A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;I6&amp;","&amp;J6&amp;","&amp;K6&amp;","&amp;L6&amp;","&amp;M6&amp;","&amp;N6&amp;","&amp;O6&amp;","&amp;P6&amp;","&amp;Q6&amp;","&amp;R6&amp;","&amp;S6&amp;","&amp;T6&amp;","&amp;U6&amp;","&amp;V6&amp;","&amp;W6&amp;","&amp;X6&amp;","&amp;Y6&amp;","&amp;Z6&amp;","&amp;AA6&amp;","&amp;AB6&amp;","&amp;AC6&amp;","&amp;AD6&amp;","&amp;AE6&amp;","&amp;AF6&amp;","&amp;AG6&amp;","&amp;AH6&amp;","&amp;AI6)</f>
+        <v>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,44,42,51,52,53,54,55,57,58,56,59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>CONCATENATE(A7&amp;","&amp;B7&amp;","&amp;C7&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;Q7&amp;","&amp;R7&amp;","&amp;S7&amp;","&amp;T7&amp;","&amp;U7&amp;","&amp;V7&amp;","&amp;W7&amp;","&amp;X7&amp;","&amp;Y7&amp;","&amp;Z7&amp;","&amp;AA7&amp;","&amp;AB7&amp;","&amp;AC7&amp;","&amp;AD7&amp;","&amp;AE7&amp;","&amp;AF7&amp;","&amp;AG7&amp;","&amp;AH7&amp;","&amp;AI7)</f>
+        <v>T2N  R13W,T1N  R16W,T1N  R14W,T2N  R15W,T4N  R12W,T4N  R15W,T2N  R16W,T1N  R11W,T3N  R14W,T3N  R12W,T4N  R16W,T1N  R15W,T4N  R11W,T3N  R15W,T2N  R11W,T3N  R13W,T1N  R12W,T4N  R14W,T4N  R13W,T3N  R16W,T1N  R13W,T2N  R14W,T2N  R12W,T3N  R11W,,,,,,,,,,,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>CONCATENATE(A8&amp;","&amp;B8&amp;","&amp;C8&amp;","&amp;D8&amp;","&amp;E8&amp;","&amp;F8&amp;","&amp;G8&amp;","&amp;H8&amp;","&amp;I8&amp;","&amp;J8&amp;","&amp;K8&amp;","&amp;L8&amp;","&amp;M8&amp;","&amp;N8&amp;","&amp;O8&amp;","&amp;P8&amp;","&amp;Q8&amp;","&amp;R8&amp;","&amp;S8&amp;","&amp;T8&amp;","&amp;U8&amp;","&amp;V8&amp;","&amp;W8&amp;","&amp;X8&amp;","&amp;Y8&amp;","&amp;Z8&amp;","&amp;AA8&amp;","&amp;AB8&amp;","&amp;AC8&amp;","&amp;AD8&amp;","&amp;AE8&amp;","&amp;AF8&amp;","&amp;AG8&amp;","&amp;AH8&amp;","&amp;AI8)</f>
+        <v>Allegan Township,Casco Township,Cheshire Township,Clyde Township,Dorr Township,Fillmore Township,Ganges Township,Gun Plain Township,Heath Township,Hopkins Township,Laketown Township,Lee Township,Leighton Township,Manlius Township,Martin Township,Monterey Township,Otsego Township,Overisel Township,Salem Township,Saugatuck Township,Trowbridge Township,Valley Township,Watson Township,Wayland Township,Hopkins Village,Martin Village,Allegan City,Fennville City,Holland City,Otsego City,Plainwell City,Saugatuck City,South Haven City,Wayland City,Douglas City</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>CONCATENATE(A9&amp;","&amp;B9&amp;","&amp;C9&amp;","&amp;D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;L9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;O9&amp;","&amp;P9&amp;","&amp;Q9&amp;","&amp;R9&amp;","&amp;S9&amp;","&amp;T9&amp;","&amp;U9&amp;","&amp;V9&amp;","&amp;W9&amp;","&amp;X9&amp;","&amp;Y9&amp;","&amp;Z9&amp;","&amp;AA9&amp;","&amp;AB9&amp;","&amp;AC9&amp;","&amp;AD9&amp;","&amp;AE9&amp;","&amp;AF9&amp;","&amp;AG9&amp;","&amp;AH9&amp;","&amp;AI9)</f>
+        <v>Allegan,Casco,Cheshire,Clyde,Dorr,Fillmore,Ganges,Gun Plain,Heath,Hopkins,Laketown,Lee,Leighton,Manlius,Martin,Monterey,Otsego,Overisel,Salem,Saugatucl,Trowbridge,Valley,Watson,Wayland,Hopkins,Martin,Allegan,Fennville,Holland,Otsego,Plainwell,Saugatuck,South Haven,Wayland,Douglas</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>CONCATENATE(A10&amp;","&amp;B10&amp;","&amp;C10&amp;","&amp;D10&amp;","&amp;E10&amp;","&amp;F10&amp;","&amp;G10&amp;","&amp;H10&amp;","&amp;I10&amp;","&amp;J10&amp;","&amp;K10&amp;","&amp;L10&amp;","&amp;M10&amp;","&amp;N10&amp;","&amp;O10&amp;","&amp;P10&amp;","&amp;Q10&amp;","&amp;R10&amp;","&amp;S10&amp;","&amp;T10&amp;","&amp;U10&amp;","&amp;V10&amp;","&amp;W10&amp;","&amp;X10&amp;","&amp;Y10&amp;","&amp;Z10&amp;","&amp;AA10&amp;","&amp;AB10&amp;","&amp;AC10&amp;","&amp;AD10&amp;","&amp;AE10&amp;","&amp;AF10&amp;","&amp;AG10&amp;","&amp;AH10&amp;","&amp;AI10)</f>
+        <v>Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Township,Village,Village,City,City,City,City,City,City,City,City,City</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>915</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -30073,1315 +31538,1547 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E1:M35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection sqref="A1:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>916</v>
+      </c>
+      <c r="B1" t="str">
+        <f>CONCATENATE("self.unit"&amp;G1&amp;" = unit"&amp;G1)</f>
+        <v>self.unit01 = unit01</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>809</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="2">
+      <c r="K1" s="2">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>917</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B33" si="0">CONCATENATE("self.unit"&amp;G2&amp;" = unit"&amp;G2)</f>
+        <v>self.unit02 = unit02</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="13">
+      <c r="H2" s="13">
         <v>13700</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="5">
+      <c r="K2" s="5">
         <v>2</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>791</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>793</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>918</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit03 = unit03</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="13">
+      <c r="H3" s="13">
         <v>15200</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="5">
+      <c r="K3" s="5">
         <v>3</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>738</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>919</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit04 = unit04</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="13">
+      <c r="H4" s="13">
         <v>16720</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="5">
+      <c r="K4" s="5">
         <v>4</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>770</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>772</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>920</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit05 = unit05</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="13">
+      <c r="H5" s="13">
         <v>22680</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="5">
+      <c r="K5" s="5">
         <v>5</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>725</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>921</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit06 = unit06</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="13">
+      <c r="H6" s="13">
         <v>28120</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="5">
+      <c r="K6" s="5">
         <v>6</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>922</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit07 = unit07</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="13">
+      <c r="H7" s="13">
         <v>31360</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>784</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="5">
+      <c r="K7" s="5">
         <v>7</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>923</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit08 = unit08</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="13">
+      <c r="H8" s="13">
         <v>35720</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="5">
+      <c r="K8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>924</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit09 = unit09</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="13">
+      <c r="H9" s="13">
         <v>37460</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="5">
+      <c r="K9" s="5">
         <v>9</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>709</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="O9" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>925</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit10 = unit10</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="G10" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="13">
+      <c r="H10" s="13">
         <v>39200</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="5">
+      <c r="K10" s="5">
         <v>10</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>750</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="O10" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>926</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit11 = unit11</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="13">
+      <c r="H11" s="13">
         <v>45180</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="5">
+      <c r="K11" s="5">
         <v>11</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>780</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>781</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="O11" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>927</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit12 = unit12</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="13">
+      <c r="H12" s="13">
         <v>46600</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="5">
+      <c r="K12" s="5">
         <v>12</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>741</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>742</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="O12" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>928</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit13 = unit13</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="13">
+      <c r="H13" s="13">
         <v>46760</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>759</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="5">
+      <c r="K13" s="5">
         <v>13</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>761</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>762</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="O13" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>929</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit14 = unit14</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="13">
+      <c r="H14" s="13">
         <v>50840</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="5">
+      <c r="K14" s="5">
         <v>14</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>767</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>768</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>930</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit15 = unit15</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="13">
+      <c r="H15" s="13">
         <v>52000</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>746</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="5">
+      <c r="K15" s="5">
         <v>15</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>748</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="N15" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="O15" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>931</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit16 = unit16</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G16" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="13">
+      <c r="H16" s="13">
         <v>55200</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="5">
+      <c r="K16" s="5">
         <v>16</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>691</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>692</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="N16" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="O16" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>932</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit17 = unit17</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="G17" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="13">
+      <c r="H17" s="13">
         <v>61640</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>775</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="5">
+      <c r="K17" s="5">
         <v>17</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="N17" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="O17" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>933</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit18 = unit18</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="G18" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="13">
+      <c r="H18" s="13">
         <v>61820</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>727</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="5">
+      <c r="K18" s="5">
         <v>18</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="O18" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>934</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit19 = unit19</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="13">
+      <c r="H19" s="13">
         <v>71100</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>702</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I19" s="5">
+      <c r="K19" s="5">
         <v>19</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>705</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="O19" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>935</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit20 = unit20</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="13">
+      <c r="H20" s="13">
         <v>71720</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>798</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="5">
+      <c r="K20" s="5">
         <v>20</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="M20" s="5" t="s">
         <v>800</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="N20" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="O20" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>936</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit21 = unit21</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="13">
+      <c r="H21" s="13">
         <v>80620</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>715</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="5">
+      <c r="K21" s="5">
         <v>21</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>716</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="O21" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>937</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit22 = unit22</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="13">
+      <c r="H22" s="13">
         <v>81580</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>731</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="5">
+      <c r="K22" s="5">
         <v>22</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="M22" s="5" t="s">
         <v>733</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="N22" s="5" t="s">
         <v>734</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="O22" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>938</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit23 = unit23</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="13">
+      <c r="H23" s="13">
         <v>84580</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="5">
+      <c r="K23" s="5">
         <v>23</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="M23" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="N23" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="O23" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>939</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit24 = unit24</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="G24" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="13">
+      <c r="H24" s="13">
         <v>84900</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="5">
+      <c r="K24" s="5">
         <v>24</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>757</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>758</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="N24" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="O24" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>940</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit42 = unit42</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="G25" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="13">
+      <c r="H25" s="13">
         <v>39200</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="I25" s="5">
+      <c r="K25" s="5">
         <v>44</v>
       </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5" t="s">
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
         <v>749</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="N25" s="5" t="s">
         <v>750</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="O25" s="6" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>941</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit44 = unit44</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="G26" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="13">
+      <c r="H26" s="13">
         <v>52000</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="I26" s="5">
+      <c r="K26" s="5">
         <v>42</v>
       </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5"/>
+      <c r="M26" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="N26" s="5" t="s">
         <v>744</v>
       </c>
-      <c r="M26" s="6" t="s">
+      <c r="O26" s="6" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>942</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit51 = unit51</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="G27" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="H27" s="13" t="s">
         <v>808</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I27" s="5">
+      <c r="K27" s="5">
         <v>51</v>
       </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5" t="s">
+      <c r="L27" s="5"/>
+      <c r="M27" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="N27" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="O27" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>943</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit52 = unit52</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="G28" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="13">
+      <c r="H28" s="13">
         <v>27740</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I28" s="5">
+      <c r="K28" s="5">
         <v>52</v>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5"/>
+      <c r="M28" s="5" t="s">
         <v>763</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="N28" s="5" t="s">
         <v>764</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="O28" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>944</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit53 = unit53</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>810</v>
       </c>
-      <c r="F29" s="13">
+      <c r="H29" s="13">
         <v>38640</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="I29" s="5">
+      <c r="K29" s="5">
         <v>53</v>
       </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5"/>
+      <c r="M29" s="5" t="s">
         <v>804</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="N29" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="O29" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>945</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit54 = unit54</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="G30" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="13">
+      <c r="H30" s="13">
         <v>61620</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="5">
+      <c r="K30" s="5">
         <v>54</v>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5" t="s">
+      <c r="L30" s="5"/>
+      <c r="M30" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="N30" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>946</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit55 = unit55</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="G31" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="13">
+      <c r="H31" s="13">
         <v>64740</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="I31" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="5">
+      <c r="K31" s="5">
         <v>55</v>
       </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5" t="s">
+      <c r="L31" s="5"/>
+      <c r="M31" s="5" t="s">
         <v>773</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="N31" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="O31" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>947</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit56 = unit56</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="G32" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F32" s="13">
+      <c r="H32" s="13">
         <v>71700</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="5">
+      <c r="K32" s="5">
         <v>57</v>
       </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5" t="s">
+      <c r="L32" s="5"/>
+      <c r="M32" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="N32" s="5" t="s">
         <v>803</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="O32" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>948</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>self.unit57 = unit57</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="E33" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="G33" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="13">
+      <c r="H33" s="13">
         <v>74980</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="I33" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="I33" s="5">
+      <c r="K33" s="5">
         <v>58</v>
       </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5" t="s">
+      <c r="L33" s="5"/>
+      <c r="M33" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="N33" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="O33" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E34" s="12" t="s">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G34" s="12" t="s">
         <v>811</v>
       </c>
-      <c r="F34" s="13">
+      <c r="H34" s="13">
         <v>84880</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="I34" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I34" s="5">
+      <c r="K34" s="5">
         <v>56</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5"/>
+      <c r="M34" s="5" t="s">
         <v>754</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="N34" s="5" t="s">
         <v>755</v>
       </c>
-      <c r="M34" s="6" t="s">
+      <c r="O34" s="6" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="14" t="s">
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="F35" s="15">
+      <c r="H35" s="15">
         <v>22740</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="I35" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="J35" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I35" s="8">
+      <c r="K35" s="8">
         <v>59</v>
       </c>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8" t="s">
+      <c r="L35" s="8"/>
+      <c r="M35" s="8" t="s">
         <v>782</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="N35" s="8" t="s">
         <v>783</v>
       </c>
-      <c r="M35" s="9" t="s">
+      <c r="O35" s="9" t="s">
         <v>697</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:B33" numberStoredAsText="1"/>
+    <ignoredError sqref="D1:D33" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>